<commit_message>
Added in links that work by changing textContent to innerHTML
</commit_message>
<xml_diff>
--- a/jsonGenerator.xlsx
+++ b/jsonGenerator.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Documents\GitHub\ChancePrayerSelection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F51FAF02-A68C-40D4-80E6-60D16094CE0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E423088E-4FEB-45BE-B625-9506C53177C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{99FF55E7-0EFB-42A1-999B-099DF6A720F8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{99FF55E7-0EFB-42A1-999B-099DF6A720F8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="26">
   <si>
     <t>name</t>
   </si>
@@ -63,9 +63,6 @@
     <t>ARRR (ARGT)</t>
   </si>
   <si>
-    <t>Go to sacredspace.ie.</t>
-  </si>
-  <si>
     <t>Imaginative Prayer</t>
   </si>
   <si>
@@ -111,10 +108,16 @@
     <t>Comtemplate</t>
   </si>
   <si>
-    <t>Imagine</t>
-  </si>
-  <si>
     <t>Praise, Repent, Ask, Yeild</t>
+  </si>
+  <si>
+    <t>Go to &lt;a href='sacredspace.ie'&gt;Sacred Space&lt;/a&gt;.</t>
+  </si>
+  <si>
+    <t>Go to &lt;a href='https://www.jesuits.org/spirituality/the-ignatian-examen/'&gt;Ignatian Examen&lt;/a&gt;.</t>
+  </si>
+  <si>
+    <t>Imagine one of the visible scenes in Scripture.</t>
   </si>
 </sst>
 </file>
@@ -469,7 +472,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4410CEAC-1B1C-4C09-90A7-E52072240D1A}">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E12" sqref="A1:E12"/>
     </sheetView>
   </sheetViews>
@@ -477,12 +480,12 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2" t="str">
         <f>_xlfn.CONCAT(Sheet2!A$1,":",quotes,Sheet2!A2,quotes,",")</f>
@@ -490,18 +493,18 @@
       </c>
       <c r="C2" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$1,":",quotes,Sheet2!B2,quotes)</f>
-        <v>description:"Go to sacredspace.ie."</v>
+        <v>description:"Go to &lt;a href='sacredspace.ie'&gt;Sacred Space&lt;/a&gt;."</v>
       </c>
       <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B3" t="str">
         <f>_xlfn.CONCAT(Sheet2!A$1,":",quotes,Sheet2!A3,quotes,",")</f>
@@ -512,15 +515,15 @@
         <v>description:"Say a simple prayer"</v>
       </c>
       <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4" t="str">
         <f>_xlfn.CONCAT(Sheet2!A$1,":",quotes,Sheet2!A4,quotes,",")</f>
@@ -528,18 +531,18 @@
       </c>
       <c r="C4" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$1,":",quotes,Sheet2!B4,quotes)</f>
-        <v>description:""</v>
+        <v>description:"Go to &lt;a href='https://www.jesuits.org/spirituality/the-ignatian-examen/'&gt;Ignatian Examen&lt;/a&gt;."</v>
       </c>
       <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B5" t="str">
         <f>_xlfn.CONCAT(Sheet2!A$1,":",quotes,Sheet2!A5,quotes,",")</f>
@@ -550,15 +553,15 @@
         <v>description:"Lectio, oratio, meditatio, contemplatio"</v>
       </c>
       <c r="D5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6" t="str">
         <f>_xlfn.CONCAT(Sheet2!A$1,":",quotes,Sheet2!A6,quotes,",")</f>
@@ -569,15 +572,15 @@
         <v>description:"Acknowledge, Relate, Receive, Respond"</v>
       </c>
       <c r="D6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B7" t="str">
         <f>_xlfn.CONCAT(Sheet2!A$1,":",quotes,Sheet2!A7,quotes,",")</f>
@@ -588,15 +591,15 @@
         <v>description:"Meditate"</v>
       </c>
       <c r="D7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B8" t="str">
         <f>_xlfn.CONCAT(Sheet2!A$1,":",quotes,Sheet2!A8,quotes,",")</f>
@@ -607,15 +610,15 @@
         <v>description:"Comtemplate"</v>
       </c>
       <c r="D8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B9" t="str">
         <f>_xlfn.CONCAT(Sheet2!A$1,":",quotes,Sheet2!A9,quotes,",")</f>
@@ -623,18 +626,18 @@
       </c>
       <c r="C9" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$1,":",quotes,Sheet2!B9,quotes)</f>
-        <v>description:"Imagine"</v>
+        <v>description:"Imagine one of the visible scenes in Scripture."</v>
       </c>
       <c r="D9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B10" t="str">
         <f>_xlfn.CONCAT(Sheet2!A$1,":",quotes,Sheet2!A10,quotes,",")</f>
@@ -645,13 +648,13 @@
         <v>description:"Praise, Repent, Ask, Yeild"</v>
       </c>
       <c r="D10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E10" s="1"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -664,8 +667,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D27C5CB6-DA7E-47DA-A5B0-1A884DEAD381}">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -678,7 +681,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -686,7 +689,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -694,20 +697,23 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
+      <c r="B4" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -715,39 +721,39 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>